<commit_message>
Added test for time dependent GBM pricer.
</commit_message>
<xml_diff>
--- a/tests/atm-volatility-surface.xlsx
+++ b/tests/atm-volatility-surface.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\gbm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4234764F-8378-475B-A46D-95CB91EAB8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BB43D4-3963-46FB-9371-AE57D337E338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18000" windowHeight="9360" xr2:uid="{1FF0D0CD-0DEF-4A06-8C4A-EBD387622EDD}"/>
   </bookViews>
   <sheets>
     <sheet name="constant_vol_surface" sheetId="2" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="B3" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="B4" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -558,7 +558,7 @@
         <v>0.25</v>
       </c>
       <c r="B5" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -567,7 +567,7 @@
         <v>0.5</v>
       </c>
       <c r="B6" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>0.75</v>
       </c>
       <c r="B7" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -592,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -600,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -624,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="5">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>